<commit_message>
fixed some stuff in the IN12 BOM
</commit_message>
<xml_diff>
--- a/rev_b/hdw/IN12_carrier/IN12_carrier/in12_carrier_bom.xlsx
+++ b/rev_b/hdw/IN12_carrier/IN12_carrier/in12_carrier_bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drew Maatman\Documents\KiCad Projects\Projects\Nixie_Clock\rev_b\hdw\IN12_carrier\IN12_carrier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A5FDCC-15F3-4997-BC7E-EDA8E6D0F532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2F0EF5-166A-4209-BAF4-08AC0E9BDA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="111">
   <si>
     <t>References</t>
   </si>
@@ -142,9 +142,6 @@
     <t>MK1101 MK1102 MK1103 MK1104 MK1105 MK1106 MK1109 MK1110 MK1111 MK1112 MK1113 MK1114 MK1117 MK1118 MK1119 MK1120 MK1121 MK1122 MK1125 MK1126 MK1127 MK1128 MK1129 MK1130</t>
   </si>
   <si>
-    <t>1772-2080-ND 1772-1220-ND</t>
-  </si>
-  <si>
     <t>Q401 Q402 Q403 Q407 Q408 Q409 Q501 Q502 Q503 Q504 Q505 Q506 Q507 Q508 Q509 Q510 Q511 Q512 Q513 Q514 Q515</t>
   </si>
   <si>
@@ -241,9 +238,6 @@
     <t>470k</t>
   </si>
   <si>
-    <t>541-470KCCT-ND Digi-Key PN: 541-470KCCT-ND</t>
-  </si>
-  <si>
     <t>R304</t>
   </si>
   <si>
@@ -323,6 +317,42 @@
   </si>
   <si>
     <t>296-44537-1-ND</t>
+  </si>
+  <si>
+    <t>541-470KCCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1772-2080-ND </t>
+  </si>
+  <si>
+    <t>1772-1220-ND</t>
+  </si>
+  <si>
+    <t>SAM8931-ND</t>
+  </si>
+  <si>
+    <t>MK1001</t>
+  </si>
+  <si>
+    <t>Pushbutton Cable</t>
+  </si>
+  <si>
+    <t>MK1002 MK1003 MK1004 MK1005 MK1006</t>
+  </si>
+  <si>
+    <t>Pushbuttons</t>
+  </si>
+  <si>
+    <t>36-7600-ND</t>
+  </si>
+  <si>
+    <t>MK1101</t>
+  </si>
+  <si>
+    <t>Feet</t>
+  </si>
+  <si>
+    <t>SJ5523-0-ND</t>
   </si>
 </sst>
 </file>
@@ -1163,11 +1193,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1378,348 +1406,404 @@
         <v>38</v>
       </c>
       <c r="E12">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="F12" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E13">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F13" t="s">
-        <v>44</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14">
+        <v>21</v>
+      </c>
+      <c r="F14" t="s">
         <v>43</v>
-      </c>
-      <c r="E14">
-        <v>6</v>
-      </c>
-      <c r="F14" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15">
-        <v>499</v>
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
       </c>
       <c r="D15" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E15">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" t="s">
-        <v>52</v>
+        <v>47</v>
+      </c>
+      <c r="B16">
+        <v>499</v>
       </c>
       <c r="D16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16">
+        <v>17</v>
+      </c>
+      <c r="F16" t="s">
         <v>49</v>
-      </c>
-      <c r="E16">
-        <v>3</v>
-      </c>
-      <c r="F16" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F17" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18">
+        <v>6</v>
+      </c>
+      <c r="F18" t="s">
         <v>55</v>
-      </c>
-      <c r="C18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18">
-        <v>3</v>
-      </c>
-      <c r="F18" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19" t="s">
         <v>55</v>
-      </c>
-      <c r="D19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19">
-        <v>21</v>
-      </c>
-      <c r="F19" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20">
+        <v>21</v>
+      </c>
+      <c r="F20" t="s">
         <v>55</v>
-      </c>
-      <c r="D20" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20">
-        <v>4</v>
-      </c>
-      <c r="F20" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D21" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21" t="s">
         <v>60</v>
-      </c>
-      <c r="E21">
-        <v>7</v>
-      </c>
-      <c r="F21" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E22">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F22" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>69</v>
-      </c>
-      <c r="C23" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="D23" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F23" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>68</v>
+      </c>
+      <c r="C24" t="s">
+        <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="E24">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
-      </c>
-      <c r="C25" t="s">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="D25" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="F25" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>73</v>
+      </c>
+      <c r="C26" t="s">
+        <v>14</v>
       </c>
       <c r="D26" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D27" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E27">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
-      </c>
-      <c r="C28" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="D28" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F28" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
+        <v>83</v>
+      </c>
+      <c r="C29" t="s">
+        <v>14</v>
       </c>
       <c r="D29" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E29">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B30" t="s">
-        <v>93</v>
-      </c>
-      <c r="C30" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="D30" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F30" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B31" t="s">
-        <v>97</v>
+        <v>91</v>
+      </c>
+      <c r="C31" t="s">
+        <v>14</v>
       </c>
       <c r="D31" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E31">
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>100</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" t="s">
+        <v>97</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" t="s">
+        <v>104</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" t="s">
+        <v>106</v>
+      </c>
+      <c r="E34">
+        <v>5</v>
+      </c>
+      <c r="F34" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>108</v>
+      </c>
+      <c r="B35" t="s">
+        <v>109</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>